<commit_message>
working logic - but data-provider is only running test for first row
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/testdata/Automation_testData.xlsx
+++ b/src/main/java/org/example/testdata/Automation_testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanda\IdeaProjects\SDETCaseStudy-1\src\main\java\org\example\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A187C8-8C9F-4EB1-8431-F5798A8BC6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FEB92A-4291-4C02-857B-F9E492520F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="630" windowWidth="14775" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,12 +127,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
     <t>ASw32$1</t>
   </si>
   <si>
@@ -149,6 +143,12 @@
   </si>
   <si>
     <t>IJLKJIKJJHKH</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
   </si>
 </sst>
 </file>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7914480-E3D9-49CD-B1C0-5D2A215DFC19}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -602,7 +602,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -614,7 +614,7 @@
         <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
         <v>24</v>
@@ -629,13 +629,13 @@
         <v>1996</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="M2">
         <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
@@ -673,13 +673,13 @@
         <v>1995</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="M3">
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>